<commit_message>
placment for grid and configManager
</commit_message>
<xml_diff>
--- a/config/layout/screen0Elements.xlsx
+++ b/config/layout/screen0Elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Python\FinanceManager\config\layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268526BF-A2EE-4D9C-B964-0BA3528955E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAFE8B2-2371-4A1D-B692-E7BB633CE0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>grid</t>
+  </si>
+  <si>
+    <t>placement</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -483,22 +492,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="14.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="14.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,14 +529,17 @@
       <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -544,19 +556,20 @@
         <v>4</v>
       </c>
       <c r="F2" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="2">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -573,15 +586,15 @@
         <v>4</v>
       </c>
       <c r="F3" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>0</v>
       </c>
     </row>
@@ -592,15 +605,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150871EB-4912-4180-B17C-83A3764DC5B5}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,14 +635,17 @@
       <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -646,19 +662,22 @@
         <v>2</v>
       </c>
       <c r="F2" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -675,19 +694,22 @@
         <v>3</v>
       </c>
       <c r="F3" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -704,15 +726,15 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
         <v>13</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2</v>
       </c>
     </row>
@@ -723,20 +745,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE39240A-12A4-4004-804D-1FFC1D0724A4}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -758,17 +780,20 @@
       <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -785,22 +810,25 @@
         <v>2</v>
       </c>
       <c r="F2" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G2" s="2">
-        <v>4</v>
-      </c>
-      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2">
         <v>30</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>100</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -817,18 +845,21 @@
         <v>3</v>
       </c>
       <c r="F3" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1">
-        <v>4</v>
-      </c>
-      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3">
         <v>30</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>100</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>0</v>
       </c>
     </row>
@@ -842,7 +873,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,7 +899,7 @@
         <v>24</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -876,7 +907,7 @@
         <v>25</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
buttons added to screen 2
</commit_message>
<xml_diff>
--- a/config/layout/screen0Elements.xlsx
+++ b/config/layout/screen0Elements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Python\FinanceManager\config\layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAFE8B2-2371-4A1D-B692-E7BB633CE0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CCBE7D-B9B0-40CA-B032-8236DF7EA9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>id</t>
   </si>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t>Password :</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>width</t>
   </si>
   <si>
     <t>textBoxType</t>
@@ -518,19 +512,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
@@ -541,7 +535,7 @@
     </row>
     <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2">
         <v>480</v>
@@ -563,7 +557,7 @@
       </c>
       <c r="H2" s="2"/>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J2" s="2">
         <v>0</v>
@@ -571,7 +565,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>580</v>
@@ -592,7 +586,7 @@
         <v>7</v>
       </c>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -624,19 +618,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
@@ -647,7 +641,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2">
         <v>480</v>
@@ -668,7 +662,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
         <v>6</v>
@@ -679,7 +673,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>470</v>
@@ -700,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -711,7 +705,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>200</v>
@@ -732,7 +726,7 @@
         <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -745,20 +739,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE39240A-12A4-4004-804D-1FFC1D0724A4}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -769,33 +762,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>550</v>
@@ -816,21 +803,15 @@
         <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2">
-        <v>30</v>
-      </c>
-      <c r="J2">
-        <v>100</v>
-      </c>
-      <c r="K2" s="2">
+        <v>32</v>
+      </c>
+      <c r="I2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>550</v>
@@ -851,15 +832,9 @@
         <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3">
-        <v>30</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
-      </c>
-      <c r="K3" s="1">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1">
         <v>0</v>
       </c>
     </row>
@@ -880,23 +855,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -904,7 +879,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>10</v>
@@ -912,10 +887,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>